<commit_message>
indicadores e aula Loinc
</commit_message>
<xml_diff>
--- a/Gestão do Projeto/Indicadores/MonitoramentoCargaOBM.xlsx
+++ b/Gestão do Projeto/Indicadores/MonitoramentoCargaOBM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatrizdefarialeao/Documents/GitHub/ips-brasil-documentos/Gestão do Projeto/Indicadores/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatrizdefarialeao/Documents/GitHub/ips-brasil-documentos/Gestão do Projeto/Indicadores/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0951A8C-CE2F-1D4D-AC3C-FD806B1B8116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448E3E48-371B-844A-A312-81F63A13469B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="26680" windowHeight="10900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14600" yWindow="2280" windowWidth="26680" windowHeight="10900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -559,7 +559,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I14"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -669,26 +669,26 @@
         <v>4799</v>
       </c>
       <c r="C6" s="1">
-        <v>1385</v>
+        <v>1100</v>
       </c>
       <c r="D6" s="2">
         <f>C6/B6</f>
-        <v>0.28860179204000835</v>
+        <v>0.22921441967076475</v>
       </c>
       <c r="E6" s="1">
-        <v>0</v>
+        <v>184</v>
       </c>
       <c r="F6" s="1">
         <v>79</v>
       </c>
       <c r="G6" s="1">
-        <v>305</v>
+        <v>656</v>
       </c>
       <c r="H6" s="1">
-        <v>850</v>
+        <v>1702</v>
       </c>
       <c r="I6" s="1">
-        <v>1223</v>
+        <v>4084</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -791,12 +791,12 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1">
         <f>SUM(C5:C13)</f>
-        <v>2540</v>
+        <v>2255</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1">
         <f t="shared" ref="E14:I14" si="0">SUM(E5:E13)</f>
-        <v>93</v>
+        <v>277</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="0"/>
@@ -804,15 +804,15 @@
       </c>
       <c r="G14" s="1">
         <f t="shared" si="0"/>
-        <v>850</v>
+        <v>1201</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>2352</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="0"/>
-        <v>1819</v>
+        <v>4680</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Indicadores Plano de Trabalho
</commit_message>
<xml_diff>
--- a/Gestão do Projeto/Indicadores/MonitoramentoCargaOBM.xlsx
+++ b/Gestão do Projeto/Indicadores/MonitoramentoCargaOBM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatrizdefarialeao/Documents/GitHub/ips-brasil-documentos/Gestão do Projeto/Indicadores/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F669AEB-E38D-F447-8E6E-7D8EB1187381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52914CC-7A92-D24F-A7BE-21EC80109E8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3560" yWindow="2280" windowWidth="26680" windowHeight="10900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2940" yWindow="760" windowWidth="26680" windowHeight="10900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>HORUS</t>
   </si>
@@ -556,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection sqref="A1:J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -642,8 +642,8 @@
         <v>1155</v>
       </c>
       <c r="D5" s="2">
-        <f>C5/B5</f>
-        <v>0.24067514065430298</v>
+        <f>(C5+C4)/4799</f>
+        <v>0.25817878724734322</v>
       </c>
       <c r="E5" s="1">
         <v>93</v>
@@ -672,8 +672,8 @@
         <v>1100</v>
       </c>
       <c r="D6" s="2">
-        <f>C14/B6</f>
-        <v>0.46988956032506773</v>
+        <f>(C6+C5+C4)/4799</f>
+        <v>0.48739320691810795</v>
       </c>
       <c r="E6" s="1">
         <v>184</v>
@@ -695,21 +695,38 @@
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="2"/>
+      <c r="B7" s="1">
+        <v>4799</v>
+      </c>
+      <c r="C7" s="1">
+        <v>481</v>
+      </c>
+      <c r="D7" s="2">
+        <f>(C7+C6+C5+C4)/B14</f>
+        <v>0.58762242133777876</v>
+      </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+      <c r="F7" s="1">
+        <v>61</v>
+      </c>
+      <c r="G7" s="1">
+        <v>298</v>
+      </c>
+      <c r="H7" s="1">
+        <v>720</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1965</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="D8" s="2"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -788,31 +805,40 @@
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="1"/>
+      <c r="B14" s="1">
+        <v>4799</v>
+      </c>
       <c r="C14" s="1">
-        <f>SUM(C5:C13)</f>
-        <v>2255</v>
-      </c>
-      <c r="D14" s="1"/>
+        <f>SUM(C4:C13)</f>
+        <v>2820</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.58762242133777876</v>
+      </c>
       <c r="E14" s="1">
         <f t="shared" ref="E14:I14" si="0">SUM(E5:E13)</f>
         <v>277</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="0"/>
-        <v>172</v>
+        <v>233</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" si="0"/>
-        <v>1201</v>
+        <v>1499</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" si="0"/>
-        <v>2352</v>
+        <v>3072</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="0"/>
-        <v>4680</v>
+        <v>6645</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
results-specimen-type-uv-ips  carga value set
</commit_message>
<xml_diff>
--- a/Gestão do Projeto/Indicadores/MonitoramentoCargaOBM.xlsx
+++ b/Gestão do Projeto/Indicadores/MonitoramentoCargaOBM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatrizdefarialeao/Documents/GitHub/ips-brasil-documentos/Gestão do Projeto/Indicadores/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE3EE9B-6AE3-2A4A-8A39-972A08236931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0911B956-76FA-A943-A556-7E99C4E11EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2940" yWindow="760" windowWidth="26680" windowHeight="10900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>HORUS</t>
   </si>
@@ -177,13 +177,13 @@
     <t>% VISTOS HÓRUS</t>
   </si>
   <si>
-    <t>VMP Incluídos Portal</t>
-  </si>
-  <si>
     <t>VMP incluídos Portal</t>
   </si>
   <si>
     <t>VMPP incluídos Portal</t>
+  </si>
+  <si>
+    <t>% VMPs incluídos no portal</t>
   </si>
 </sst>
 </file>
@@ -252,11 +252,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:K14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -616,14 +614,14 @@
       <c r="I3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -739,7 +737,9 @@
         <f>(C7+C6+C5+C4)/B14</f>
         <v>0.90560533444467595</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
       <c r="F7" s="1">
         <v>61</v>
       </c>
@@ -754,27 +754,47 @@
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-      <c r="L7" s="1">
-        <v>136</v>
-      </c>
+      <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
+      <c r="B8" s="1">
+        <v>4799</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4799</v>
+      </c>
+      <c r="D8" s="2">
+        <f>(C8)/B14</f>
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1013</v>
+      </c>
+      <c r="H8" s="1">
+        <v>850</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1223</v>
+      </c>
+      <c r="J8">
+        <v>434</v>
+      </c>
+      <c r="K8" s="4">
+        <f>J8/B8</f>
+        <v>9.0435507397374451E-2</v>
+      </c>
+      <c r="L8">
+        <v>1307</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -856,9 +876,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
-      <c r="L13" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
@@ -868,12 +886,11 @@
         <v>4799</v>
       </c>
       <c r="C14" s="1">
-        <f>SUM(C4:C13)</f>
-        <v>4346</v>
+        <v>4799</v>
       </c>
       <c r="D14" s="2">
         <f>C14/B14</f>
-        <v>0.90560533444467595</v>
+        <v>1</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" ref="E14" si="0">SUM(E5:E13)</f>
@@ -881,26 +898,28 @@
       </c>
       <c r="F14" s="1">
         <f>SUM(F4:F13)</f>
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="G14" s="1">
         <f>SUM(G4:G13)</f>
-        <v>1532</v>
+        <v>2545</v>
       </c>
       <c r="H14" s="1">
         <f>SUM(H4:H13)</f>
-        <v>3256</v>
+        <v>4106</v>
       </c>
       <c r="I14" s="1">
         <f>SUM(I4:I13)</f>
-        <v>6701</v>
-      </c>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1">
-        <f>SUM(L5:L13)</f>
-        <v>136</v>
-      </c>
+        <v>7924</v>
+      </c>
+      <c r="J14" s="1">
+        <v>434</v>
+      </c>
+      <c r="K14" s="2">
+        <f>J14/B14</f>
+        <v>9.0435507397374451E-2</v>
+      </c>
+      <c r="L14" s="1"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D15" t="s">

</xml_diff>